<commit_message>
reading optimized with pydantic
</commit_message>
<xml_diff>
--- a/tests/fixtures/ApstraProvisiongTemplate.xlsx
+++ b/tests/fixtures/ApstraProvisiongTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckim/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckim/Documents/Projects/panda-test-001/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF4C103-CE00-8B4A-9C46-6A02766E5874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E39D25-942E-9C47-A644-449FD1BCE7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="-17360" windowWidth="29940" windowHeight="16360" xr2:uid="{1E8E1A00-D519-B44D-83B4-6FFC064194AF}"/>
+    <workbookView xWindow="4160" yWindow="-35740" windowWidth="34220" windowHeight="15440" xr2:uid="{1E8E1A00-D519-B44D-83B4-6FFC064194AF}"/>
   </bookViews>
   <sheets>
     <sheet name="generic_systems" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>blueprint</t>
   </si>
@@ -47,18 +47,9 @@
     <t>switch1</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>ifname</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
-    <t>blah</t>
-  </si>
-  <si>
     <t>atl1tor-r5r6a</t>
   </si>
   <si>
@@ -89,18 +80,12 @@
     <t>comment</t>
   </si>
   <si>
-    <t>track_info</t>
-  </si>
-  <si>
     <t>lag_mode</t>
   </si>
   <si>
     <t>is_external</t>
   </si>
   <si>
-    <t>gs_ifname</t>
-  </si>
-  <si>
     <t>switch2</t>
   </si>
   <si>
@@ -120,12 +105,84 @@
   </si>
   <si>
     <t>et-0/0/3-b</t>
+  </si>
+  <si>
+    <t>testtag</t>
+  </si>
+  <si>
+    <t>lacp_active</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ct_names</t>
+  </si>
+  <si>
+    <t>connectivity_template</t>
+  </si>
+  <si>
+    <t>blah-1</t>
+  </si>
+  <si>
+    <t>sys001</t>
+  </si>
+  <si>
+    <t>10G</t>
+  </si>
+  <si>
+    <t>blah-2</t>
+  </si>
+  <si>
+    <t>leaf2</t>
+  </si>
+  <si>
+    <t>xe-0/0/6</t>
+  </si>
+  <si>
+    <t>label1</t>
+  </si>
+  <si>
+    <t>ifname1</t>
+  </si>
+  <si>
+    <t>gs_ifname1</t>
+  </si>
+  <si>
+    <t>label2</t>
+  </si>
+  <si>
+    <t>ifname2</t>
+  </si>
+  <si>
+    <t>gs_ifname2</t>
+  </si>
+  <si>
+    <t>label3</t>
+  </si>
+  <si>
+    <t>ifname3</t>
+  </si>
+  <si>
+    <t>gs_ifname3</t>
+  </si>
+  <si>
+    <t>label4</t>
+  </si>
+  <si>
+    <t>ifname4</t>
+  </si>
+  <si>
+    <t>gs_ifname4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -173,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -210,7 +267,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -228,7 +285,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -243,21 +300,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -273,7 +315,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -288,13 +330,35 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -303,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -319,26 +383,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,247 +728,282 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="5" customWidth="1"/>
-    <col min="12" max="13" width="13.5" style="5" customWidth="1"/>
-    <col min="14" max="16" width="10.83203125" style="7"/>
-    <col min="17" max="19" width="10.83203125" style="9"/>
-    <col min="20" max="20" width="12.6640625" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="5" customWidth="1"/>
+    <col min="11" max="12" width="13.5" style="5" customWidth="1"/>
+    <col min="13" max="15" width="10.83203125" style="7"/>
+    <col min="16" max="18" width="10.83203125" style="9"/>
+    <col min="19" max="19" width="14.33203125" style="26" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" style="26" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="22"/>
     </row>
     <row r="2" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21" t="s">
+      <c r="A2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:22" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="H3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="22"/>
-    </row>
-    <row r="3" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11" t="s">
+      <c r="P3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="Q1:S1"/>
+  <dataConsolidate/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tooltip" prompt="The blueprint label (name)." sqref="B1:B2" xr:uid="{771FBAAF-65D1-A44E-B8BA-65F93D6C44DD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tooltip" prompt="The generic system label (name)." sqref="C1:C2" xr:uid="{3B11CCCD-AB45-834C-A051-843486EA42B3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tooltip" prompt="Yes for the external generic system. Default is empty (no)." sqref="D1:D2" xr:uid="{830EA207-4D0D-2A48-B7F5-3B1989CA302C}"/>
+  <dataValidations count="11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="blueprint label" prompt="The name of the blueprint." sqref="A1:A2" xr:uid="{771FBAAF-65D1-A44E-B8BA-65F93D6C44DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="generic system label" prompt="The name of the generic system." sqref="B2" xr:uid="{3B11CCCD-AB45-834C-A051-843486EA42B3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is External?" prompt="Yes for the external generic system. Default is no." sqref="C2" xr:uid="{830EA207-4D0D-2A48-B7F5-3B1989CA302C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="Connectivity template names. comma separated. i.e. &quot;vn200-untagged, Template524, m-firewall1&quot;" sqref="U2" xr:uid="{33CF8FDF-4047-9942-BF2E-100BC1B3219E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="mandatory" prompt="The name of the first swich (order doesn't matter) in case of multiple memeber LAG, or the only switch." sqref="G1:I1" xr:uid="{D742E826-BC54-6C45-82B9-9C7590CCAA07}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="connectivity templates" prompt="A vlan, regardless of its connectivity name variations, should be present in only one place. " sqref="S1:U1" xr:uid="{EF656843-950B-3640-9011-1D424EC64CCA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="untagged vlan id. i.e. 55" sqref="S2" xr:uid="{4E5E686B-FDFC-624C-B15D-18CC8BEDA5AA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="Tagged vlans. i.e. &quot;35, 77, 123, 124, 1005&quot;" sqref="T2" xr:uid="{22AC89F2-8C17-1749-8719-3DCED0EC7F8D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="The name of the second swich (order doesn't matter) in case of multiple memeber LAG." sqref="J1:L1" xr:uid="{D6FCCDFB-A1F8-6C4E-9372-275FB625956A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="The name of the third swich (order doesn't matter) in case of multiple memeber LAG." sqref="M1:O1" xr:uid="{4BA0154D-616D-114A-8B51-ABC201104F70}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="optional" prompt="The name of the fourth swich (order doesn't matter) in case of multiple memeber LAG." sqref="P1:R1" xr:uid="{981FFF0D-2678-C14B-9206-1D8C3CDB5955}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>